<commit_message>
Made a change to test things are actually pulling data from this sheet properly
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1fb1801062dea39/Documents/clough/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F53C2A0-90C4-4E94-B561-7D9E9D591880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA66AE-896E-4903-A518-1B1438EF451C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +679,7 @@
         <v>45533</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Centered text in another cell to test new centering feature in Clough. It worked :)
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBA66AE-896E-4903-A518-1B1438EF451C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944EC91-F32D-4C64-BD9E-3D4BD2170AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -85,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -95,6 +95,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,7 +521,7 @@
       <c r="A10" s="2">
         <v>45513</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>2.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now handles left, right & centre horizontal alignment, aligns row labels, and defaults to right align as Excel does
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944EC91-F32D-4C64-BD9E-3D4BD2170AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FDE3D-5992-439B-B097-2A91250F2822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -85,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -98,6 +98,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,7 +439,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,7 +532,7 @@
       <c r="A11" s="2">
         <v>45514</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>14.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added italics and underlines to this sheet to detect next
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FDE3D-5992-439B-B097-2A91250F2822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D2CB84-B020-4F39-ADA1-C2326F8CB96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +58,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -85,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -101,6 +117,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +461,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +498,7 @@
       <c r="A4" s="2">
         <v>45507</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6">
         <v>12.4</v>
       </c>
     </row>
@@ -484,7 +506,7 @@
       <c r="A5" s="2">
         <v>45508</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
         <v>3.8</v>
       </c>
     </row>
@@ -492,7 +514,7 @@
       <c r="A6" s="2">
         <v>45509</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>0</v>
       </c>
     </row>
@@ -500,7 +522,7 @@
       <c r="A7" s="2">
         <v>45510</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>18.7</v>
       </c>
     </row>
@@ -698,5 +720,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now writing bold, italic and underline to font_style in cell dict
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D2CB84-B020-4F39-ADA1-C2326F8CB96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58E4FA-F8ED-45C2-A2C6-B0C74EAFBC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -122,6 +132,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -461,7 +474,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +543,7 @@
       <c r="A8" s="2">
         <v>45511</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="8">
         <v>6.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More styles to test
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE58E4FA-F8ED-45C2-A2C6-B0C74EAFBC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66743F98-EE1C-46AF-BEFA-06338DB6A9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +90,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -135,6 +162,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -473,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +619,7 @@
       <c r="A13" s="2">
         <v>45516</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="9">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -591,7 +627,7 @@
       <c r="A14" s="2">
         <v>45517</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="10">
         <v>9.1</v>
       </c>
     </row>
@@ -599,7 +635,7 @@
       <c r="A15" s="2">
         <v>45518</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stuck some extra rows of data in, for testing. Works fine
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66743F98-EE1C-46AF-BEFA-06338DB6A9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B70300-44B3-43FC-9584-0290D1D15B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -171,6 +171,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,6 +770,54 @@
         <v>11.3</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B32" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45536</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45537</v>
+      </c>
+      <c r="B34" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45538</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45539</v>
+      </c>
+      <c r="B36" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45540</v>
+      </c>
+      <c r="B37" s="12">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Got another sheet in the workbook now
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66743F98-EE1C-46AF-BEFA-06338DB6A9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33B31B7-CB0E-477D-85B7-B49DCCE7014F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Rainfall (mm)</t>
+  </si>
+  <si>
+    <t>Forgot this one</t>
   </si>
 </sst>
 </file>
@@ -507,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,6 +771,285 @@
         <v>11.3</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FEEF18-091E-4D26-8576-E9911AF3317A}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45536</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45537</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45538</v>
+      </c>
+      <c r="B4" s="6">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45539</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45540</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45541</v>
+      </c>
+      <c r="B7" s="7">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45542</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45543</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45544</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45545</v>
+      </c>
+      <c r="B11" s="5">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45546</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45547</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B14" s="10">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45549</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45550</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45551</v>
+      </c>
+      <c r="B17" s="3">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45552</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45554</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45555</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45556</v>
+      </c>
+      <c r="B22" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45557</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45558</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45559</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45560</v>
+      </c>
+      <c r="B26" s="3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45561</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45562</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45563</v>
+      </c>
+      <c r="B29" s="3">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45564</v>
+      </c>
+      <c r="B30" s="3">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Now three sheets, including one with three columns, not two
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33B31B7-CB0E-477D-85B7-B49DCCE7014F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E79D0C6-5C6A-48D6-B569-A89687DEF173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>Forgot this one</t>
+  </si>
+  <si>
+    <t>Foo</t>
   </si>
 </sst>
 </file>
@@ -142,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,6 +179,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FEEF18-091E-4D26-8576-E9911AF3317A}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,7 +809,7 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +822,7 @@
         <v>45536</v>
       </c>
       <c r="B2" s="3">
-        <v>5.2</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -820,27 +830,27 @@
         <v>45537</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="13">
         <v>45538</v>
       </c>
       <c r="B4" s="6">
-        <v>12.4</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="13">
         <v>45539</v>
       </c>
       <c r="B5" s="6">
-        <v>3.8</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="13">
         <v>45540</v>
       </c>
       <c r="B6" s="7">
@@ -848,23 +858,23 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="13">
         <v>45541</v>
       </c>
       <c r="B7" s="7">
-        <v>18.7</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="13">
         <v>45542</v>
       </c>
       <c r="B8" s="8">
-        <v>6.3</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="13">
         <v>45543</v>
       </c>
       <c r="B9" s="3">
@@ -872,19 +882,19 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="13">
         <v>45544</v>
       </c>
       <c r="B10" s="4">
-        <v>2.9</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="13">
         <v>45545</v>
       </c>
       <c r="B11" s="5">
-        <v>14.2</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -892,7 +902,7 @@
         <v>45546</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -900,7 +910,7 @@
         <v>45547</v>
       </c>
       <c r="B13" s="9">
-        <v>4.5999999999999996</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -908,7 +918,7 @@
         <v>45548</v>
       </c>
       <c r="B14" s="10">
-        <v>9.1</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -916,7 +926,7 @@
         <v>45549</v>
       </c>
       <c r="B15" s="11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -924,7 +934,7 @@
         <v>45550</v>
       </c>
       <c r="B16" s="3">
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -932,71 +942,71 @@
         <v>45551</v>
       </c>
       <c r="B17" s="3">
-        <v>23.3</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45552</v>
       </c>
-      <c r="B18" s="3">
-        <v>0</v>
+      <c r="B18" s="12">
+        <v>7.2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45553</v>
       </c>
-      <c r="B19" s="3">
-        <v>1.5</v>
+      <c r="B19" s="12">
+        <v>2.8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45554</v>
       </c>
-      <c r="B20" s="3">
-        <v>7.8</v>
+      <c r="B20" s="12">
+        <v>18.3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45555</v>
       </c>
-      <c r="B21" s="3">
-        <v>0</v>
+      <c r="B21" s="12">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45556</v>
       </c>
-      <c r="B22" s="3">
-        <v>15.6</v>
+      <c r="B22" s="12">
+        <v>15.2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45557</v>
       </c>
-      <c r="B23" s="3">
-        <v>0</v>
+      <c r="B23" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45558</v>
       </c>
-      <c r="B24" s="3">
-        <v>8.1999999999999993</v>
+      <c r="B24" s="12">
+        <v>5.8</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45559</v>
       </c>
-      <c r="B25" s="3">
-        <v>0</v>
+      <c r="B25" s="12">
+        <v>8.9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1004,7 +1014,7 @@
         <v>45560</v>
       </c>
       <c r="B26" s="3">
-        <v>13.7</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1012,7 +1022,7 @@
         <v>45561</v>
       </c>
       <c r="B27" s="3">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1028,7 +1038,7 @@
         <v>45563</v>
       </c>
       <c r="B29" s="3">
-        <v>19.399999999999999</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1036,7 +1046,7 @@
         <v>45564</v>
       </c>
       <c r="B30" s="3">
-        <v>13.5</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1044,7 +1054,7 @@
         <v>45565</v>
       </c>
       <c r="B31" s="3">
-        <v>11.3</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1054,4 +1064,371 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DA9CA6-57DD-4798-A56F-2023663C7AAB}">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45566</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45567</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45568</v>
+      </c>
+      <c r="B4" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45569</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45570</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45571</v>
+      </c>
+      <c r="B7" s="7">
+        <v>18.7</v>
+      </c>
+      <c r="C7" s="7">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45572</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6.3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45573</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45574</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45575</v>
+      </c>
+      <c r="B11" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45576</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45577</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B14" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="C14" s="10">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45579</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45580</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45581</v>
+      </c>
+      <c r="B17" s="3">
+        <v>23.3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45583</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C19" s="12">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45584</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="C20" s="12">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45585</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45586</v>
+      </c>
+      <c r="B22" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="C22" s="12">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45587</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45588</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C24" s="12">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45589</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="12">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45590</v>
+      </c>
+      <c r="B26" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="C26" s="3">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45591</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45592</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45593</v>
+      </c>
+      <c r="B29" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C29" s="3">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45594</v>
+      </c>
+      <c r="B30" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45595</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45596</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more sheets for testing
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B70300-44B3-43FC-9584-0290D1D15B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98008EA7-4C17-428C-8B16-2BD1D0D4D02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Date</t>
   </si>
@@ -512,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection sqref="A1:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,4 +824,626 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45505</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45506</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45507</v>
+      </c>
+      <c r="B4" s="6">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45508</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45509</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45510</v>
+      </c>
+      <c r="B7" s="7">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45511</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45512</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45513</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45514</v>
+      </c>
+      <c r="B11" s="5">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45515</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45516</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45517</v>
+      </c>
+      <c r="B14" s="10">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45518</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45519</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45520</v>
+      </c>
+      <c r="B17" s="3">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45521</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45522</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45523</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45524</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45525</v>
+      </c>
+      <c r="B22" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45526</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45528</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45529</v>
+      </c>
+      <c r="B26" s="3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45530</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45531</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45532</v>
+      </c>
+      <c r="B29" s="3">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45533</v>
+      </c>
+      <c r="B30" s="3">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45534</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B32" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45536</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45537</v>
+      </c>
+      <c r="B34" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45538</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45539</v>
+      </c>
+      <c r="B36" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45540</v>
+      </c>
+      <c r="B37" s="12">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD67A1F-0B1C-49A0-A2B7-EDFE6DD57055}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45505</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45506</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45507</v>
+      </c>
+      <c r="B4" s="6">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45508</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45509</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45510</v>
+      </c>
+      <c r="B7" s="7">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45511</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45512</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45513</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45514</v>
+      </c>
+      <c r="B11" s="5">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45515</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45516</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45517</v>
+      </c>
+      <c r="B14" s="10">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45518</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45519</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45520</v>
+      </c>
+      <c r="B17" s="3">
+        <v>23.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45521</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45522</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45523</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45524</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45525</v>
+      </c>
+      <c r="B22" s="3">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45526</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45528</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45529</v>
+      </c>
+      <c r="B26" s="3">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45530</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45531</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45532</v>
+      </c>
+      <c r="B29" s="3">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45533</v>
+      </c>
+      <c r="B30" s="3">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45534</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45535</v>
+      </c>
+      <c r="B32" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45536</v>
+      </c>
+      <c r="B33" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45537</v>
+      </c>
+      <c r="B34" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45538</v>
+      </c>
+      <c r="B35" s="12">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45539</v>
+      </c>
+      <c r="B36" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45540</v>
+      </c>
+      <c r="B37" s="12">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Edited other tabs so I can tell them apart
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98008EA7-4C17-428C-8B16-2BD1D0D4D02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C680AB-1035-467E-A1D9-DE8C7D294888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -38,12 +38,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Rainfall (mm)</t>
+  </si>
+  <si>
+    <t>^sppoky</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection sqref="A1:B37"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,11 +833,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -846,7 +852,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="B2" s="3">
         <v>5.2</v>
@@ -854,7 +860,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45506</v>
+        <v>45537</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -862,7 +868,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>45507</v>
+        <v>45538</v>
       </c>
       <c r="B4" s="6">
         <v>12.4</v>
@@ -870,7 +876,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>45508</v>
+        <v>45539</v>
       </c>
       <c r="B5" s="6">
         <v>3.8</v>
@@ -878,7 +884,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>45509</v>
+        <v>45540</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
@@ -886,7 +892,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>45510</v>
+        <v>45541</v>
       </c>
       <c r="B7" s="7">
         <v>18.7</v>
@@ -894,7 +900,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>45511</v>
+        <v>45542</v>
       </c>
       <c r="B8" s="8">
         <v>6.3</v>
@@ -902,7 +908,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>45512</v>
+        <v>45543</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -910,7 +916,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>45513</v>
+        <v>45544</v>
       </c>
       <c r="B10" s="4">
         <v>2.9</v>
@@ -918,7 +924,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>45514</v>
+        <v>45545</v>
       </c>
       <c r="B11" s="5">
         <v>14.2</v>
@@ -926,7 +932,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>45515</v>
+        <v>45546</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -934,7 +940,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>45516</v>
+        <v>45547</v>
       </c>
       <c r="B13" s="9">
         <v>4.5999999999999996</v>
@@ -942,7 +948,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>45517</v>
+        <v>45548</v>
       </c>
       <c r="B14" s="10">
         <v>9.1</v>
@@ -950,7 +956,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>45518</v>
+        <v>45549</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
@@ -958,7 +964,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>45519</v>
+        <v>45550</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -966,7 +972,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45520</v>
+        <v>45551</v>
       </c>
       <c r="B17" s="3">
         <v>23.3</v>
@@ -974,7 +980,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45521</v>
+        <v>45552</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -982,7 +988,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>45522</v>
+        <v>45553</v>
       </c>
       <c r="B19" s="3">
         <v>1.5</v>
@@ -990,7 +996,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>45523</v>
+        <v>45554</v>
       </c>
       <c r="B20" s="3">
         <v>7.8</v>
@@ -998,7 +1004,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>45524</v>
+        <v>45555</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -1006,7 +1012,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>45525</v>
+        <v>45556</v>
       </c>
       <c r="B22" s="3">
         <v>15.6</v>
@@ -1014,7 +1020,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>45526</v>
+        <v>45557</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -1022,7 +1028,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>45527</v>
+        <v>45558</v>
       </c>
       <c r="B24" s="3">
         <v>8.1999999999999993</v>
@@ -1030,7 +1036,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>45528</v>
+        <v>45559</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -1038,7 +1044,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>45529</v>
+        <v>45560</v>
       </c>
       <c r="B26" s="3">
         <v>13.7</v>
@@ -1046,7 +1052,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>45530</v>
+        <v>45561</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -1054,7 +1060,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>45531</v>
+        <v>45562</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -1062,7 +1068,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>45532</v>
+        <v>45563</v>
       </c>
       <c r="B29" s="3">
         <v>19.399999999999999</v>
@@ -1070,7 +1076,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>45533</v>
+        <v>45564</v>
       </c>
       <c r="B30" s="3">
         <v>13.5</v>
@@ -1078,59 +1084,35 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>45534</v>
+        <v>45565</v>
       </c>
       <c r="B31" s="3">
         <v>11.3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>45535</v>
-      </c>
-      <c r="B32" s="3">
-        <v>12.5</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>45536</v>
-      </c>
-      <c r="B33" s="12">
-        <v>1.5</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="12"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>45537</v>
-      </c>
-      <c r="B34" s="12">
-        <v>16</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>45538</v>
-      </c>
-      <c r="B35" s="12">
-        <v>2.4</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>45539</v>
-      </c>
-      <c r="B36" s="12">
-        <v>8</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="12"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>45540</v>
-      </c>
-      <c r="B37" s="12">
-        <v>7</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1141,11 +1123,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD67A1F-0B1C-49A0-A2B7-EDFE6DD57055}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1157,7 +1142,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>45505</v>
+        <v>45566</v>
       </c>
       <c r="B2" s="3">
         <v>5.2</v>
@@ -1165,7 +1150,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45506</v>
+        <v>45567</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1173,7 +1158,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>45507</v>
+        <v>45568</v>
       </c>
       <c r="B4" s="6">
         <v>12.4</v>
@@ -1181,7 +1166,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>45508</v>
+        <v>45569</v>
       </c>
       <c r="B5" s="6">
         <v>3.8</v>
@@ -1189,7 +1174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>45509</v>
+        <v>45570</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
@@ -1197,7 +1182,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>45510</v>
+        <v>45571</v>
       </c>
       <c r="B7" s="7">
         <v>18.7</v>
@@ -1205,7 +1190,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>45511</v>
+        <v>45572</v>
       </c>
       <c r="B8" s="8">
         <v>6.3</v>
@@ -1213,7 +1198,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>45512</v>
+        <v>45573</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1221,7 +1206,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>45513</v>
+        <v>45574</v>
       </c>
       <c r="B10" s="4">
         <v>2.9</v>
@@ -1229,7 +1214,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>45514</v>
+        <v>45575</v>
       </c>
       <c r="B11" s="5">
         <v>14.2</v>
@@ -1237,7 +1222,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>45515</v>
+        <v>45576</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
@@ -1245,7 +1230,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>45516</v>
+        <v>45577</v>
       </c>
       <c r="B13" s="9">
         <v>4.5999999999999996</v>
@@ -1253,7 +1238,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>45517</v>
+        <v>45578</v>
       </c>
       <c r="B14" s="10">
         <v>9.1</v>
@@ -1261,7 +1246,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>45518</v>
+        <v>45579</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
@@ -1269,7 +1254,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>45519</v>
+        <v>45580</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
@@ -1277,7 +1262,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>45520</v>
+        <v>45581</v>
       </c>
       <c r="B17" s="3">
         <v>23.3</v>
@@ -1285,7 +1270,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>45521</v>
+        <v>45582</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -1293,7 +1278,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>45522</v>
+        <v>45583</v>
       </c>
       <c r="B19" s="3">
         <v>1.5</v>
@@ -1301,7 +1286,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>45523</v>
+        <v>45584</v>
       </c>
       <c r="B20" s="3">
         <v>7.8</v>
@@ -1309,7 +1294,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>45524</v>
+        <v>45585</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -1317,7 +1302,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>45525</v>
+        <v>45586</v>
       </c>
       <c r="B22" s="3">
         <v>15.6</v>
@@ -1325,7 +1310,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>45526</v>
+        <v>45587</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -1333,7 +1318,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>45527</v>
+        <v>45588</v>
       </c>
       <c r="B24" s="3">
         <v>8.1999999999999993</v>
@@ -1341,7 +1326,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>45528</v>
+        <v>45589</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -1349,7 +1334,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>45529</v>
+        <v>45590</v>
       </c>
       <c r="B26" s="3">
         <v>13.7</v>
@@ -1357,7 +1342,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>45530</v>
+        <v>45591</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -1365,7 +1350,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>45531</v>
+        <v>45592</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -1373,7 +1358,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>45532</v>
+        <v>45593</v>
       </c>
       <c r="B29" s="3">
         <v>19.399999999999999</v>
@@ -1381,7 +1366,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>45533</v>
+        <v>45594</v>
       </c>
       <c r="B30" s="3">
         <v>13.5</v>
@@ -1389,7 +1374,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>45534</v>
+        <v>45595</v>
       </c>
       <c r="B31" s="3">
         <v>11.3</v>
@@ -1397,51 +1382,33 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>45535</v>
+        <v>45596</v>
       </c>
       <c r="B32" s="3">
         <v>12.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>45536</v>
-      </c>
-      <c r="B33" s="12">
-        <v>1.5</v>
-      </c>
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="12"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>45537</v>
-      </c>
-      <c r="B34" s="12">
-        <v>16</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>45538</v>
-      </c>
-      <c r="B35" s="12">
-        <v>2.4</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>45539</v>
-      </c>
-      <c r="B36" s="12">
-        <v>8</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="12"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>45540</v>
-      </c>
-      <c r="B37" s="12">
-        <v>7</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made the spreadsheet a bit more complicated
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C680AB-1035-467E-A1D9-DE8C7D294888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D4BA70-01A7-47A2-AE37-7190FBD009F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="MySheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Rainfall (mm)</t>
   </si>
   <si>
-    <t>^sppoky</t>
+    <t>How I'm feeling about that</t>
+  </si>
+  <si>
+    <t>^sppooaky</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1121,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD67A1F-0B1C-49A0-A2B7-EDFE6DD57055}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,267 +1135,363 @@
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45566</v>
       </c>
       <c r="B2" s="3">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45567</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45568</v>
       </c>
       <c r="B4" s="6">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45569</v>
       </c>
       <c r="B5" s="6">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45570</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45571</v>
       </c>
       <c r="B7" s="7">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45572</v>
       </c>
       <c r="B8" s="8">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45573</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45574</v>
       </c>
       <c r="B10" s="4">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45575</v>
       </c>
       <c r="B11" s="5">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45577</v>
       </c>
       <c r="B13" s="9">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45578</v>
       </c>
       <c r="B14" s="10">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45579</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45580</v>
       </c>
       <c r="B16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45581</v>
       </c>
       <c r="B17" s="3">
         <v>23.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45582</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45583</v>
       </c>
       <c r="B19" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45584</v>
       </c>
       <c r="B20" s="3">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45585</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45586</v>
       </c>
       <c r="B22" s="3">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45587</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45588</v>
       </c>
       <c r="B24" s="3">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45589</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45590</v>
       </c>
       <c r="B26" s="3">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45591</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45592</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45593</v>
       </c>
       <c r="B29" s="3">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45594</v>
       </c>
       <c r="B30" s="3">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45595</v>
       </c>
       <c r="B31" s="3">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45596</v>
       </c>
       <c r="B32" s="3">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="12"/>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>

</xml_diff>

<commit_message>
Edited to remove some rows etc for testing
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D4BA70-01A7-47A2-AE37-7190FBD009F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79FAA8-5B3A-4F19-A9A0-5D39F9E2E82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="MySheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -834,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,30 +1092,6 @@
       <c r="B31" s="3">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="12"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="12"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More data to test sideways scrolling
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC79FAA8-5B3A-4F19-A9A0-5D39F9E2E82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B12966-A787-4A2A-954D-318B2753ADD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,36 @@
   </si>
   <si>
     <t>^sppooaky</t>
+  </si>
+  <si>
+    <t>Foo1</t>
+  </si>
+  <si>
+    <t>Foo2</t>
+  </si>
+  <si>
+    <t>Foo3</t>
+  </si>
+  <si>
+    <t>Foo4</t>
+  </si>
+  <si>
+    <t>Foo5</t>
+  </si>
+  <si>
+    <t>Foo6</t>
+  </si>
+  <si>
+    <t>Foo7</t>
+  </si>
+  <si>
+    <t>Foo8</t>
+  </si>
+  <si>
+    <t>Foo9</t>
+  </si>
+  <si>
+    <t>Foo10</t>
   </si>
 </sst>
 </file>
@@ -836,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
@@ -1100,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD67A1F-0B1C-49A0-A2B7-EDFE6DD57055}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,7 +1141,7 @@
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,8 +1151,38 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45566</v>
       </c>
@@ -1132,8 +1192,38 @@
       <c r="C2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45567</v>
       </c>
@@ -1143,8 +1233,38 @@
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45568</v>
       </c>
@@ -1154,8 +1274,38 @@
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45569</v>
       </c>
@@ -1165,8 +1315,38 @@
       <c r="C5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45570</v>
       </c>
@@ -1176,8 +1356,38 @@
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45571</v>
       </c>
@@ -1187,8 +1397,38 @@
       <c r="C7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45572</v>
       </c>
@@ -1198,8 +1438,38 @@
       <c r="C8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45573</v>
       </c>
@@ -1209,8 +1479,38 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45574</v>
       </c>
@@ -1220,8 +1520,38 @@
       <c r="C10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45575</v>
       </c>
@@ -1231,8 +1561,38 @@
       <c r="C11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
@@ -1242,8 +1602,38 @@
       <c r="C12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>11</v>
+      </c>
+      <c r="M12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45577</v>
       </c>
@@ -1253,8 +1643,38 @@
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45578</v>
       </c>
@@ -1264,8 +1684,38 @@
       <c r="C14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>13</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45579</v>
       </c>
@@ -1275,8 +1725,38 @@
       <c r="C15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>14</v>
+      </c>
+      <c r="M15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45580</v>
       </c>
@@ -1286,8 +1766,38 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
+      </c>
+      <c r="M16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45581</v>
       </c>
@@ -1297,8 +1807,38 @@
       <c r="C17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>16</v>
+      </c>
+      <c r="M17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45582</v>
       </c>
@@ -1308,8 +1848,38 @@
       <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>17</v>
+      </c>
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <v>17</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="L18">
+        <v>17</v>
+      </c>
+      <c r="M18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45583</v>
       </c>
@@ -1319,8 +1889,38 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+      <c r="L19">
+        <v>18</v>
+      </c>
+      <c r="M19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45584</v>
       </c>
@@ -1330,8 +1930,38 @@
       <c r="C20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>19</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>19</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+      <c r="L20">
+        <v>19</v>
+      </c>
+      <c r="M20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45585</v>
       </c>
@@ -1341,8 +1971,38 @@
       <c r="C21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>20</v>
+      </c>
+      <c r="M21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45586</v>
       </c>
@@ -1352,8 +2012,38 @@
       <c r="C22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>21</v>
+      </c>
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>21</v>
+      </c>
+      <c r="K22">
+        <v>21</v>
+      </c>
+      <c r="L22">
+        <v>21</v>
+      </c>
+      <c r="M22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45587</v>
       </c>
@@ -1363,8 +2053,38 @@
       <c r="C23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23">
+        <v>22</v>
+      </c>
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23">
+        <v>22</v>
+      </c>
+      <c r="K23">
+        <v>22</v>
+      </c>
+      <c r="L23">
+        <v>22</v>
+      </c>
+      <c r="M23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45588</v>
       </c>
@@ -1374,8 +2094,38 @@
       <c r="C24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24">
+        <v>23</v>
+      </c>
+      <c r="K24">
+        <v>23</v>
+      </c>
+      <c r="L24">
+        <v>23</v>
+      </c>
+      <c r="M24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45589</v>
       </c>
@@ -1385,8 +2135,38 @@
       <c r="C25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <v>24</v>
+      </c>
+      <c r="K25">
+        <v>24</v>
+      </c>
+      <c r="L25">
+        <v>24</v>
+      </c>
+      <c r="M25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45590</v>
       </c>
@@ -1396,8 +2176,38 @@
       <c r="C26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>25</v>
+      </c>
+      <c r="K26">
+        <v>25</v>
+      </c>
+      <c r="L26">
+        <v>25</v>
+      </c>
+      <c r="M26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45591</v>
       </c>
@@ -1407,8 +2217,38 @@
       <c r="C27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27">
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <v>26</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27">
+        <v>26</v>
+      </c>
+      <c r="K27">
+        <v>26</v>
+      </c>
+      <c r="L27">
+        <v>26</v>
+      </c>
+      <c r="M27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45592</v>
       </c>
@@ -1418,8 +2258,38 @@
       <c r="C28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <v>27</v>
+      </c>
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>27</v>
+      </c>
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>27</v>
+      </c>
+      <c r="K28">
+        <v>27</v>
+      </c>
+      <c r="L28">
+        <v>27</v>
+      </c>
+      <c r="M28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45593</v>
       </c>
@@ -1429,8 +2299,38 @@
       <c r="C29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <v>28</v>
+      </c>
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>28</v>
+      </c>
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29">
+        <v>28</v>
+      </c>
+      <c r="K29">
+        <v>28</v>
+      </c>
+      <c r="L29">
+        <v>28</v>
+      </c>
+      <c r="M29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45594</v>
       </c>
@@ -1440,8 +2340,38 @@
       <c r="C30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="J30">
+        <v>29</v>
+      </c>
+      <c r="K30">
+        <v>29</v>
+      </c>
+      <c r="L30">
+        <v>29</v>
+      </c>
+      <c r="M30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45595</v>
       </c>
@@ -1451,8 +2381,38 @@
       <c r="C31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>30</v>
+      </c>
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="J31">
+        <v>30</v>
+      </c>
+      <c r="K31">
+        <v>30</v>
+      </c>
+      <c r="L31">
+        <v>30</v>
+      </c>
+      <c r="M31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45596</v>
       </c>
@@ -1462,26 +2422,116 @@
       <c r="C32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>31</v>
+      </c>
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32">
+        <v>31</v>
+      </c>
+      <c r="I32">
+        <v>31</v>
+      </c>
+      <c r="J32">
+        <v>31</v>
+      </c>
+      <c r="K32">
+        <v>31</v>
+      </c>
+      <c r="L32">
+        <v>31</v>
+      </c>
+      <c r="M32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>32</v>
+      </c>
+      <c r="K33">
+        <v>32</v>
+      </c>
+      <c r="L33">
+        <v>32</v>
+      </c>
+      <c r="M33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <v>33</v>
+      </c>
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>33</v>
+      </c>
+      <c r="I34">
+        <v>33</v>
+      </c>
+      <c r="J34">
+        <v>33</v>
+      </c>
+      <c r="K34">
+        <v>33</v>
+      </c>
+      <c r="L34">
+        <v>33</v>
+      </c>
+      <c r="M34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="12"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="12"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="12"/>
     </row>

</xml_diff>

<commit_message>
Now uses the apply_number_formatting module cos direct conversion from Excel's number formats is a mess
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE46E00-2C89-41BD-89F7-D033599AF5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2B2FA-7037-46DD-8A01-A69D8CE02727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +680,7 @@
         <v>45505</v>
       </c>
       <c r="B2" s="13">
-        <v>5.2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added handling for British short dates i.e. DD/MM/YY
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD2B2FA-7037-46DD-8A01-A69D8CE02727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82F7828-9431-4F3B-B4A9-96DFE5D2864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Second sheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -149,6 +149,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,6 +322,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -657,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC36EAA-0A74-4B01-A126-00D4C8F5DE27}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -973,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE23BDE-4696-4E23-9522-81A5FA1262C7}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,7 +997,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="16">
         <v>45536</v>
       </c>
       <c r="B2" s="3">
@@ -999,7 +1005,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="16">
         <v>45537</v>
       </c>
       <c r="B3" s="3">
@@ -1007,7 +1013,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="16">
         <v>45538</v>
       </c>
       <c r="B4" s="6">
@@ -1015,7 +1021,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="16">
         <v>45539</v>
       </c>
       <c r="B5" s="6">
@@ -1023,7 +1029,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="16">
         <v>45540</v>
       </c>
       <c r="B6" s="7">
@@ -1031,7 +1037,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="16">
         <v>45541</v>
       </c>
       <c r="B7" s="7">
@@ -1039,7 +1045,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="16">
         <v>45542</v>
       </c>
       <c r="B8" s="8">
@@ -1047,7 +1053,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="16">
         <v>45543</v>
       </c>
       <c r="B9" s="3">
@@ -1055,7 +1061,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="16">
         <v>45544</v>
       </c>
       <c r="B10" s="4">
@@ -1063,7 +1069,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="16">
         <v>45545</v>
       </c>
       <c r="B11" s="5">
@@ -1239,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD67A1F-0B1C-49A0-A2B7-EDFE6DD57055}">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AG1" sqref="AG1:AH1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying some more number formats
</commit_message>
<xml_diff>
--- a/test_data/test_sheet_01.xlsx
+++ b/test_data/test_sheet_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjtho\Documents\clough\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82F7828-9431-4F3B-B4A9-96DFE5D2864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99239911-8035-4833-B75F-FA4EAEB7E226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5ACD8E0-32AF-4BC9-B649-D9CAC7FA328C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -144,13 +144,16 @@
   <si>
     <t>Foo31</t>
   </si>
+  <si>
+    <t>$4.50</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -277,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,9 +327,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1246,7 +1250,7 @@
   <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AH1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,8 +1372,8 @@
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>35</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1472,8 +1476,8 @@
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" s="17">
+        <v>5.75</v>
       </c>
       <c r="E3">
         <v>2</v>

</xml_diff>